<commit_message>
added tasks to documentacija.
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Support: Linkai i support ir help puslapius</t>
   </si>
   <si>
-    <t>Support + Help: Search laukelio likimas</t>
-  </si>
-  <si>
     <t>Favouritebooks: Pilka erdve</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>HelpCenter: mintis ateičiai - video į jutiūbą</t>
   </si>
   <si>
-    <t>BuyBooks: Turi tokį pat funkcionalumą kaip vaizdas "Browse"... Išspręsti šitą klausimą.</t>
-  </si>
-  <si>
     <t>Wishlist: Kažkaip ne taip pagal reikalavimus, nei kad padarėme...</t>
   </si>
   <si>
@@ -109,13 +103,52 @@
   </si>
   <si>
     <t>Pereiti per validatorių</t>
+  </si>
+  <si>
+    <t>Nuimti bjauria spalva</t>
+  </si>
+  <si>
+    <t>Help/Support puslapiai - linkai isave neveikia.</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Wishlist: Mygtukai dideli truputi mazesni, o mazieji - didesni, bet vienoje linijoje.</t>
+  </si>
+  <si>
+    <t>Birute</t>
+  </si>
+  <si>
+    <t>MyBookApp pakeisti i BookStore</t>
+  </si>
+  <si>
+    <t>Registration/login: maziau balts spalvos + apvalus kampuciai visos formos</t>
+  </si>
+  <si>
+    <t>REACT: Paruosia susinstalinimo ir pazintini kelia, parodo maza pvz, kaip tai igyvendinama (kaip is html persikelti i REACT).</t>
+  </si>
+  <si>
+    <t>Aurimas</t>
+  </si>
+  <si>
+    <t>Sukurti saugu kelia githube, kad ant masterio butu galima daryti naujus pakeitimus.</t>
+  </si>
+  <si>
+    <t>Support + Help: Search laukelio likimas - istrinti</t>
+  </si>
+  <si>
+    <t>BuyBooks: Turi tokį pat funkcionalumą kaip vaizdas "Browse"... Išspręsti šitą klausimą. Sprendimas: Klientas neteisus. Paaiskinsim klientui, kaip turi būti.</t>
+  </si>
+  <si>
+    <t>Jurgis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -204,17 +237,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -288,6 +329,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -322,6 +364,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -497,14 +540,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
@@ -514,7 +557,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -531,439 +574,538 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7">
+        <v>43116</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="30">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>27</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="B18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="B19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="B20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="B23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -975,24 +1117,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Smth small updated in darbai list
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -543,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,6 +586,9 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Started login and register forms :)
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,54 @@
   </si>
   <si>
     <t>Jurgis</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Wishlist subheader</t>
+  </si>
+  <si>
+    <t>BuyBooks subheader</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>SuppoertContacts</t>
+  </si>
+  <si>
+    <t>REACT: Footer</t>
+  </si>
+  <si>
+    <t>REACT: Wishlist subheader</t>
+  </si>
+  <si>
+    <t>REACT: BuyBooks subheader</t>
+  </si>
+  <si>
+    <t>REACT: Login</t>
+  </si>
+  <si>
+    <t>REACT: Register</t>
+  </si>
+  <si>
+    <t>REACT: Support Contacts</t>
+  </si>
+  <si>
+    <t>REACT: Knygos vienos erdve</t>
+  </si>
+  <si>
+    <t>REACT: Sulipdyti i viena erdve, kur keicias viduriai</t>
+  </si>
+  <si>
+    <t>Knygos: Kaip turi atrodyti paduodama info su knygomis</t>
+  </si>
+  <si>
+    <t>clear: both;</t>
   </si>
 </sst>
 </file>
@@ -541,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,7 +700,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>33</v>
@@ -669,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
@@ -795,6 +843,9 @@
       <c r="B16" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
@@ -802,13 +853,16 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>41</v>
       </c>
@@ -816,7 +870,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -824,13 +878,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>19</v>
       </c>
@@ -838,7 +895,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -848,30 +905,39 @@
       <c r="D20" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="C23" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>24</v>
       </c>
@@ -879,12 +945,12 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -892,7 +958,7 @@
         <v>36</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>37</v>
@@ -901,7 +967,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -909,7 +975,7 @@
         <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
@@ -917,113 +983,215 @@
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J26" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="7">
+        <v>43118</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="7">
+        <v>43118</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="7">
+        <v>43118</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="7">
+        <v>43118</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="7">
+        <v>43118</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
BuyBooks ir wishlist isvaizda sutvarkyta. Atnaujintas darbu sarasiukas isskiriant CSS dali.
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CSStaisymas" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -190,13 +190,49 @@
   </si>
   <si>
     <t>clear: both;</t>
+  </si>
+  <si>
+    <t>Vieta</t>
+  </si>
+  <si>
+    <t>BuyBooks</t>
+  </si>
+  <si>
+    <t>Visas</t>
+  </si>
+  <si>
+    <t>Tuščia erdvė prieš footerį</t>
+  </si>
+  <si>
+    <t>Favourites</t>
+  </si>
+  <si>
+    <t>Tekstas nuo mygtukų nušoko</t>
+  </si>
+  <si>
+    <t>Wishlist</t>
+  </si>
+  <si>
+    <t>Foto ir teksto dydis, tekstas nušokęs po foto</t>
+  </si>
+  <si>
+    <t>Login neveikia (neišmeta lentelės)</t>
+  </si>
+  <si>
+    <t>Visur</t>
+  </si>
+  <si>
+    <t>Kiekio ir kainos laukelių spalva į whitesmoke</t>
+  </si>
+  <si>
+    <t>Pav kamapai neapvalinti.. Ar apvalinti..?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,7 +326,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -303,7 +339,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -377,7 +413,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -412,7 +447,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -588,14 +622,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
@@ -605,7 +639,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -625,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -642,7 +676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -662,7 +696,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -673,7 +707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -684,7 +718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -692,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -709,7 +743,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="30">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -726,7 +760,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -743,7 +777,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="26.25" customHeight="1">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -751,7 +785,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -768,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="30">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -785,7 +819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -802,7 +836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -819,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -836,7 +870,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -853,7 +887,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -870,7 +904,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -878,7 +912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -895,7 +929,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="30">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -909,7 +943,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -923,12 +957,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="30">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -945,12 +979,12 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -967,7 +1001,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -987,7 +1021,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1004,7 +1038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1021,7 +1055,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1038,7 +1072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1055,7 +1089,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1072,7 +1106,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1089,7 +1123,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1103,7 +1137,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1117,7 +1151,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1131,152 +1165,152 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5">
       <c r="A48" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1">
       <c r="A49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1">
       <c r="A50" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1">
       <c r="A51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1">
       <c r="A52" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1">
       <c r="A53" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1">
       <c r="A54" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1">
       <c r="A55" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1">
       <c r="A56" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1">
       <c r="A57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1">
       <c r="A58" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1">
       <c r="A59" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1288,24 +1322,371 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F55"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26.25" customHeight="1">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Atnaujintas CSS darbu sarasas
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="CSStaisymas" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CSStaisymas!$A$1:$E$55</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -190,6 +193,86 @@
   </si>
   <si>
     <t>clear: both;</t>
+  </si>
+  <si>
+    <t>Vieta</t>
+  </si>
+  <si>
+    <t>BuyBooks</t>
+  </si>
+  <si>
+    <t>Visas</t>
+  </si>
+  <si>
+    <t>Favourites</t>
+  </si>
+  <si>
+    <t>Tekstas nuo mygtukų nušoko</t>
+  </si>
+  <si>
+    <t>Wishlist</t>
+  </si>
+  <si>
+    <t>Foto ir teksto dydis, tekstas nušokęs po foto</t>
+  </si>
+  <si>
+    <t>Login neveikia (neišmeta lentelės)</t>
+  </si>
+  <si>
+    <t>Visur</t>
+  </si>
+  <si>
+    <t>Kiekio ir kainos laukelių spalva į whitesmoke</t>
+  </si>
+  <si>
+    <t>Pav kamapai neapvalinti.. Ar apvalinti..?</t>
+  </si>
+  <si>
+    <t>Dingo pavadinimai</t>
+  </si>
+  <si>
+    <t>Cursorius ant mygtuku kad pirstukas</t>
+  </si>
+  <si>
+    <t>Cursiorius ant paspaustu mygtuku - pagriebra rankele</t>
+  </si>
+  <si>
+    <t>Help center FireFox prie kazkokio vienintelio zoomo susikrenta kaip nereikia</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Browse</t>
+  </si>
+  <si>
+    <t>Bookgrid - nuimti scrola, kai nera pakankamai daug knygu, jis turi isnykti.</t>
+  </si>
+  <si>
+    <t>Login neveikia (mygtuko paspaudimas)</t>
+  </si>
+  <si>
+    <t>Subheader plotis skiriasi visuose psl</t>
+  </si>
+  <si>
+    <t>Subheader tarpelis tarp total price ir mygtuko Buy</t>
+  </si>
+  <si>
+    <t>Tuščia erdvė prieš footerį:
+ - 780 scrollbaro nustatymas gride
+ - amount divas issoka uz bendro knygos divo aukscio</t>
+  </si>
+  <si>
+    <t>Rizika, kad gali tekti perdaryti +- mygtukus, nes jie buttons</t>
+  </si>
+  <si>
+    <t>Linija is subheaderio</t>
+  </si>
+  <si>
+    <t>Subheadery yra nusokus lupa (gali but susije su linija)</t>
+  </si>
+  <si>
+    <t>Prio4</t>
   </si>
 </sst>
 </file>
@@ -591,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,6 +1218,9 @@
       <c r="A36" s="2">
         <v>35</v>
       </c>
+      <c r="B36" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -1289,13 +1375,459 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E55">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
created function to switch login/register state from shown to hiden, added function to calculate total price of chart
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
@@ -11,12 +11,15 @@
     <sheet name="CSStaisymas" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CSStaisymas!$A$1:$E$55</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
   <si>
     <t>ID</t>
   </si>
@@ -201,9 +204,6 @@
     <t>Visas</t>
   </si>
   <si>
-    <t>Tuščia erdvė prieš footerį</t>
-  </si>
-  <si>
     <t>Favourites</t>
   </si>
   <si>
@@ -226,13 +226,60 @@
   </si>
   <si>
     <t>Pav kamapai neapvalinti.. Ar apvalinti..?</t>
+  </si>
+  <si>
+    <t>Dingo pavadinimai</t>
+  </si>
+  <si>
+    <t>Cursorius ant mygtuku kad pirstukas</t>
+  </si>
+  <si>
+    <t>Cursiorius ant paspaustu mygtuku - pagriebra rankele</t>
+  </si>
+  <si>
+    <t>Help center FireFox prie kazkokio vienintelio zoomo susikrenta kaip nereikia</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Browse</t>
+  </si>
+  <si>
+    <t>Bookgrid - nuimti scrola, kai nera pakankamai daug knygu, jis turi isnykti.</t>
+  </si>
+  <si>
+    <t>Login neveikia (mygtuko paspaudimas)</t>
+  </si>
+  <si>
+    <t>Subheader plotis skiriasi visuose psl</t>
+  </si>
+  <si>
+    <t>Subheader tarpelis tarp total price ir mygtuko Buy</t>
+  </si>
+  <si>
+    <t>Tuščia erdvė prieš footerį:
+ - 780 scrollbaro nustatymas gride
+ - amount divas issoka uz bendro knygos divo aukscio</t>
+  </si>
+  <si>
+    <t>Rizika, kad gali tekti perdaryti +- mygtukus, nes jie buttons</t>
+  </si>
+  <si>
+    <t>Linija is subheaderio</t>
+  </si>
+  <si>
+    <t>Subheadery yra nusokus lupa (gali but susije su linija)</t>
+  </si>
+  <si>
+    <t>Prio4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,7 +373,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -339,7 +386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -413,6 +460,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -447,6 +495,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,14 +671,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
@@ -639,7 +688,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -659,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -676,7 +725,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -696,7 +745,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -707,7 +756,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -718,7 +767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -726,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="45">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -743,7 +792,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -760,7 +809,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -777,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26.25" customHeight="1">
+    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -785,7 +834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -802,7 +851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -819,7 +868,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -836,7 +885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -853,7 +902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -870,7 +919,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="30">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -887,7 +936,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -904,7 +953,7 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -912,7 +961,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -929,7 +978,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -943,7 +992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -957,12 +1006,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="30">
+    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -979,12 +1028,12 @@
         <v>43116</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45">
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1001,7 +1050,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30">
+    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1021,7 +1070,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1038,7 +1087,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1055,7 +1104,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1072,7 +1121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1089,7 +1138,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1106,7 +1155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1123,7 +1172,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1137,7 +1186,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1151,7 +1200,7 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1165,152 +1214,155 @@
         <v>43118</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="B36" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -1322,14 +1374,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
@@ -1338,7 +1391,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1356,12 +1409,12 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>59</v>
@@ -1373,48 +1426,51 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>33</v>
@@ -1423,270 +1479,365 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="B8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" customHeight="1">
+      <c r="B9" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="B10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="B11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="B12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="B13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="B14" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="B15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E55">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CSS:  - Tarpas tarp booterio ir grid - patvarkytas
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -258,21 +258,25 @@
     <t>Subheader tarpelis tarp total price ir mygtuko Buy</t>
   </si>
   <si>
+    <t>Rizika, kad gali tekti perdaryti +- mygtukus, nes jie buttons</t>
+  </si>
+  <si>
+    <t>Linija is subheaderio</t>
+  </si>
+  <si>
+    <t>Subheadery yra nusokus lupa (gali but susije su linija)</t>
+  </si>
+  <si>
+    <t>Prio4</t>
+  </si>
+  <si>
     <t>Tuščia erdvė prieš footerį:
- - 780 scrollbaro nustatymas gride
- - amount divas issoka uz bendro knygos divo aukscio</t>
-  </si>
-  <si>
-    <t>Rizika, kad gali tekti perdaryti +- mygtukus, nes jie buttons</t>
-  </si>
-  <si>
-    <t>Linija is subheaderio</t>
-  </si>
-  <si>
-    <t>Subheadery yra nusokus lupa (gali but susije su linija)</t>
-  </si>
-  <si>
-    <t>Prio4</t>
+ - Gali būti, kad pasistums i virsu, kai pilkas subheaderis susitvarkys. Bet dabar visuose 3 griduose padariau grid height 780&gt;700 ir 730&gt;700.
+Dar possible problema: amount divas issoka uz bendro knygos divo aukscio</t>
+  </si>
+  <si>
+    <t>Testavimas, 
+neradau kur istrinti knygas is buybooks saraso</t>
   </si>
 </sst>
 </file>
@@ -348,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -370,6 +374,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1378,7 +1385,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,18 +1432,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1542,7 +1552,7 @@
         <v>73</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1550,7 +1560,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>74</v>
@@ -1606,13 +1616,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>59</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,7 +1630,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
BuyBooks: 	- Solved issue with missing book title
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -13,13 +13,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">CSStaisymas!$A$1:$E$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$65</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
   <si>
     <t>ID</t>
   </si>
@@ -73,9 +74,6 @@
   </si>
   <si>
     <t>Support: Pridėti email laukelį prie laiško formos + šviesiai pilgas headeris (ten sukelti temas)</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
   <si>
     <t>Daniel</t>
@@ -275,8 +273,10 @@
 Dar possible problema: amount divas issoka uz bendro knygos divo aukscio</t>
   </si>
   <si>
-    <t>Testavimas, 
-neradau kur istrinti knygas is buybooks saraso</t>
+    <t>Testavimas</t>
+  </si>
+  <si>
+    <t>Divinukai knygu kur yra 4, pertikrinti, kad imtu Mygtuku faila is bendro folderio, o ne is Div3.</t>
   </si>
 </sst>
 </file>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,10 +723,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
@@ -737,13 +737,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="7">
         <v>43116</v>
@@ -759,6 +759,12 @@
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
@@ -787,13 +793,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7">
         <v>43116</v>
@@ -807,10 +813,10 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="7">
         <v>43116</v>
@@ -824,10 +830,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
@@ -849,10 +855,10 @@
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -863,13 +869,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -880,13 +886,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
@@ -897,13 +903,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
@@ -914,13 +920,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -931,13 +937,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="7">
         <v>43116</v>
@@ -948,13 +954,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="7">
         <v>43116</v>
@@ -965,7 +971,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -973,13 +979,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="7">
         <v>43118</v>
@@ -990,13 +996,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="J20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -1004,21 +1010,33 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="7">
+        <v>43116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1026,55 +1044,67 @@
         <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="7">
-        <v>43116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="E25" s="7">
+        <v>43118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="E26" s="7">
+        <v>43118</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -1082,16 +1112,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E27" s="7">
         <v>43118</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -1099,16 +1132,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E28" s="7">
         <v>43118</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -1116,16 +1152,19 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="E29" s="7">
         <v>43118</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1133,16 +1172,19 @@
         <v>29</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="E30" s="7">
         <v>43118</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1150,16 +1192,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E31" s="7">
         <v>43118</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -1167,13 +1212,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E32" s="7">
         <v>43118</v>
@@ -1184,10 +1229,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="E33" s="7">
         <v>43118</v>
@@ -1198,36 +1243,24 @@
         <v>33</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="7">
-        <v>43118</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="7">
-        <v>43118</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -1375,6 +1408,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E65"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1382,10 +1416,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,7 +1428,8 @@
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1405,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>
@@ -1415,38 +1451,38 @@
       </c>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>83</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1454,10 +1490,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1465,27 +1501,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1493,13 +1532,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,10 +1546,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1518,13 +1563,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1532,27 +1577,27 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1560,27 +1605,30 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1588,13 +1636,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1602,27 +1650,30 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1630,18 +1681,21 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1830,7 +1884,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E55"/>
+  <autoFilter ref="A1:E55">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Favourites: 	- Solved issue with buttons text; 	- Small changes on small buttons styles (made a bit bigger with adjusted tect size).
Wishlist:
	- Changed buttons from normal to small.
</commit_message>
<xml_diff>
--- a/00_dokumentacija/darbai_v01.xlsx
+++ b/00_dokumentacija/darbai_v01.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="88">
   <si>
     <t>ID</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Divinukai knygu kur yra 4, pertikrinti, kad imtu Mygtuku faila is bendro folderio, o ne is Div3.</t>
+  </si>
+  <si>
+    <t>Nereik</t>
+  </si>
+  <si>
+    <t>BuyBooks ir pan.</t>
+  </si>
+  <si>
+    <t>Done, bet dar biski perdariau mygtukus wishliste</t>
   </si>
 </sst>
 </file>
@@ -1420,14 +1429,14 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="24.42578125" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
@@ -1496,7 +1505,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1508,6 +1517,9 @@
       </c>
       <c r="D5" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -1540,6 +1552,9 @@
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1571,6 +1586,9 @@
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -1585,6 +1603,9 @@
       <c r="D10" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1676,7 +1697,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1690,80 +1711,89 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1890,7 +1920,7 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>